<commit_message>
dangtq sửa đơn 3b,3c,3d
</commit_message>
<xml_diff>
--- a/Business/Trao đổi với khách hàng/Report for status.xlsx
+++ b/Business/Trao đổi với khách hàng/Report for status.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090F8FB7-FD55-4314-8E5A-5461203B393E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F1A382-47E3-44B4-AE99-9C1A11F3D0DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10995" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,14 +23,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Thư thông báo</t>
   </si>
   <si>
-    <t>Báo cáo đính kèm</t>
-  </si>
-  <si>
     <t>Trạng thái</t>
   </si>
   <si>
@@ -43,36 +40,18 @@
     <t>Acceptance Report</t>
   </si>
   <si>
-    <t>Acceptance Decision Notice</t>
-  </si>
-  <si>
     <t>App Plublication Notice</t>
   </si>
   <si>
-    <t>Application Publication</t>
-  </si>
-  <si>
     <t>Grant Notification Report</t>
   </si>
   <si>
-    <t>Notification of Allowance</t>
-  </si>
-  <si>
     <t>Recordal of change</t>
   </si>
   <si>
-    <t>Notification of recordation</t>
-  </si>
-  <si>
-    <t>Application for TM registration</t>
-  </si>
-  <si>
     <t>Renewal Filing report</t>
   </si>
   <si>
-    <t>Reviewal &amp; Change Decision</t>
-  </si>
-  <si>
     <t>Chuyển nhượng/Assignment</t>
   </si>
   <si>
@@ -94,59 +73,10 @@
     <t>Report on recordal of assignment</t>
   </si>
   <si>
-    <t>Certificate of Asignment Recordal</t>
-  </si>
-  <si>
     <t>Phản đối cấp bằng/Opposition</t>
   </si>
   <si>
     <t>Filing Advice of Opposition</t>
-  </si>
-  <si>
-    <t>Approval Notification</t>
-  </si>
-  <si>
-    <t>Tham khảo</t>
-  </si>
-  <si>
-    <t>Business\Report Form\Grant - Vietnam</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Renewal\Renewal Filing Report</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Advice of Filing</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Renewal\Renewal&amp;Change Decisions</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Opposition\Filing advice_Opposition against Minh Nhung Crocodile Shop and device.doc</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Opposition\Approval Notification_PairSONIC (English Translation).doc</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Publication of Application\Application Publication Notice_AJISEN and device.doc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">\Business\Report Form\Publication of Application\Application Publication _AJISEN and device (English Translation).doc
-</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Acceptance Decision Report\Acceptance Decision Report_ENNETSU-DROP Device.doc</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Acceptance Decision Report\Acceptance Decision_ENNETSU-DROP Device (English Translation).doc</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Assignment\Certifiacate of  Recordal of Assignment_Trademark Registration No.57550.doc</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Assignment\Report on Recordal of Assignment_Trademark Registration No.57550.doc</t>
-  </si>
-  <si>
-    <t>\Business\Report Form\Recordal_Change_Assignment</t>
   </si>
   <si>
     <t>Mỗi trạng thái đều có 1 mẫu đơn riêng,cả bản tiếng anh và tiếng việt, sau khi có kết quả của cục admin/luật sư điền kết quả từ cục -&gt; admin duyệt -&gt; send thông báo cho KH</t>
@@ -159,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,16 +104,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,18 +115,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,46 +143,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -550,231 +437,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:F15"/>
+  <dimension ref="A3:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1" t="s">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1" t="s">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" display="E:\Working\Legaltech\Business\Report Form\Renewal\Renewal Filing Report" xr:uid="{8795AA9F-FE95-4714-9964-D26FE68C36A3}"/>
-    <hyperlink ref="C8" r:id="rId2" xr:uid="{29F8C88A-DA10-472D-98C2-82D64912BED3}"/>
-    <hyperlink ref="F8" r:id="rId3" xr:uid="{74E8D232-ECDE-412A-AF36-91FE97806281}"/>
-    <hyperlink ref="F10" r:id="rId4" xr:uid="{1320BAE3-DA56-4E09-AC09-B0CE41D6F53B}"/>
-    <hyperlink ref="C7" r:id="rId5" display="\Business\Report Form\Opposition\20100429 Filing advice_Opposition against Minh Nhung Crocodile Shop and device.doc" xr:uid="{2311ED69-FFCC-42CF-A9C8-3094FB588846}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{D466D5E9-E2EB-4A78-8D63-E2011BE961A4}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{EF528A85-8F49-4D43-97D6-4C6FAF0C3DA3}"/>
-    <hyperlink ref="F6" r:id="rId8" display="..\Report Form\Publication of Application" xr:uid="{70F4AD01-E0A0-4A55-85F8-30387D719896}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{F833341C-A139-49B4-85FD-AF4924E592AF}"/>
-    <hyperlink ref="F5" r:id="rId10" xr:uid="{7656F280-BA54-449C-B457-274F7BA196FD}"/>
-    <hyperlink ref="F4" r:id="rId11" xr:uid="{22429BC5-884C-465D-B76B-B5E60F7F2A8C}"/>
-    <hyperlink ref="C4" r:id="rId12" xr:uid="{D05C230C-F72C-4E10-A99A-DC256384697A}"/>
-    <hyperlink ref="C11" r:id="rId13" xr:uid="{6723FD8D-00E0-4469-A2CA-F1690097E0AA}"/>
-    <hyperlink ref="F11" r:id="rId14" xr:uid="{6CFCD5EF-32D4-4270-975F-F61F4199EE4F}"/>
-    <hyperlink ref="F9" r:id="rId15" xr:uid="{9C5087CF-BBD3-45FD-9A4E-3025288EE03F}"/>
-    <hyperlink ref="C9" r:id="rId16" xr:uid="{C9C5744B-F847-4648-B7E7-BAC73D7BAEA9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>